<commit_message>
Fixes with setting up jRuby.
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -19,16 +19,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="131">
   <si>
-    <t>Инвентарный номер</t>
-  </si>
-  <si>
-    <t>Наименование</t>
-  </si>
-  <si>
-    <t>Число ТО за год</t>
-  </si>
-  <si>
-    <t>Норма трудоемкости, чел.*час.</t>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Number per year</t>
+  </si>
+  <si>
+    <t>Work amount</t>
   </si>
   <si>
     <t>Трудоемкость ремонта за год, чел*час.</t>
@@ -381,7 +381,7 @@
     <t>_____________ В.Е. Рыхлицкий</t>
   </si>
   <si>
-    <t>КАЛЬКУЛЯЦИЯ </t>
+    <t>КАЛЬКУЛЯЦИЯ</t>
   </si>
   <si>
     <t>на 1 час технического обслуживания</t>
@@ -402,10 +402,10 @@
     <t>Заработная плата</t>
   </si>
   <si>
-    <t>Отчисления на социальное страхование </t>
-  </si>
-  <si>
-    <t>Обязательное страхование </t>
+    <t>Отчисления на социальное страхование</t>
+  </si>
+  <si>
+    <t>Обязательное страхование</t>
   </si>
   <si>
     <t>Общехозяйственные расходы</t>
@@ -414,7 +414,7 @@
     <t>Итого себестоимость</t>
   </si>
   <si>
-    <t>Прибыль </t>
+    <t>Прибыль</t>
   </si>
   <si>
     <t>Итого стоимость с учётом прибыли</t>
@@ -423,13 +423,13 @@
     <t>Цена без учета НДС</t>
   </si>
   <si>
-    <t>НДС </t>
+    <t>НДС</t>
   </si>
   <si>
     <t>Стоимость с НДС</t>
   </si>
   <si>
-    <t>Итого: </t>
+    <t>Итого:</t>
   </si>
   <si>
     <t>НДС:</t>
@@ -448,18 +448,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-    <numFmt formatCode="0" numFmtId="166"/>
-    <numFmt formatCode="0.00" numFmtId="167"/>
-    <numFmt formatCode="#,##0" numFmtId="168"/>
+    <numFmt formatCode="0" numFmtId="165"/>
+    <numFmt formatCode="0.00" numFmtId="166"/>
+    <numFmt formatCode="#,##0" numFmtId="167"/>
   </numFmts>
   <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -653,171 +653,171 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="1" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="12" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="15" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="12" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="12" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="0" fontId="11" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="11" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="166" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="10" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="10" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="5" fillId="0" fontId="10" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="6" fillId="0" fontId="10" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="12" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="12" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="0" fontId="11" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="11" numFmtId="168" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="10" numFmtId="168" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="5" fillId="0" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="6" fillId="0" fontId="10" numFmtId="168" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="168" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="167" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="168" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="167" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -840,8 +840,8 @@
   </sheetPr>
   <dimension ref="A1:AC59"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A34" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="D57" activeCellId="0" pane="topLeft" sqref="D57"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="D8" activeCellId="0" pane="topLeft" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -878,7 +878,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="33.75" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30.55" outlineLevel="0" r="8">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Write xlsx to yml.
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -19,16 +19,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="131">
   <si>
-    <t>Инвентарный номер</t>
-  </si>
-  <si>
-    <t>Наименование</t>
-  </si>
-  <si>
-    <t>Число ТО за год</t>
-  </si>
-  <si>
-    <t>Норма трудоемкости, чел.*час.</t>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Number per year</t>
+  </si>
+  <si>
+    <t>Work amount</t>
   </si>
   <si>
     <t>Трудоемкость ремонта за год, чел*час.</t>
@@ -363,7 +363,7 @@
     <t>Шкаф холодильный СМ 110, шт</t>
   </si>
   <si>
-    <t>ИТОГО:</t>
+    <t>RESULT:</t>
   </si>
   <si>
     <t>оклад</t>
@@ -381,7 +381,7 @@
     <t>_____________ В.Е. Рыхлицкий</t>
   </si>
   <si>
-    <t>КАЛЬКУЛЯЦИЯ </t>
+    <t>КАЛЬКУЛЯЦИЯ</t>
   </si>
   <si>
     <t>на 1 час технического обслуживания</t>
@@ -402,10 +402,10 @@
     <t>Заработная плата</t>
   </si>
   <si>
-    <t>Отчисления на социальное страхование </t>
-  </si>
-  <si>
-    <t>Обязательное страхование </t>
+    <t>Отчисления на социальное страхование</t>
+  </si>
+  <si>
+    <t>Обязательное страхование</t>
   </si>
   <si>
     <t>Общехозяйственные расходы</t>
@@ -414,7 +414,7 @@
     <t>Итого себестоимость</t>
   </si>
   <si>
-    <t>Прибыль </t>
+    <t>Прибыль</t>
   </si>
   <si>
     <t>Итого стоимость с учётом прибыли</t>
@@ -423,13 +423,13 @@
     <t>Цена без учета НДС</t>
   </si>
   <si>
-    <t>НДС </t>
+    <t>НДС</t>
   </si>
   <si>
     <t>Стоимость с НДС</t>
   </si>
   <si>
-    <t>Итого: </t>
+    <t>Итого:</t>
   </si>
   <si>
     <t>НДС:</t>
@@ -448,18 +448,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-    <numFmt formatCode="0" numFmtId="166"/>
-    <numFmt formatCode="0.00" numFmtId="167"/>
-    <numFmt formatCode="#,##0" numFmtId="168"/>
+    <numFmt formatCode="0" numFmtId="165"/>
+    <numFmt formatCode="0.00" numFmtId="166"/>
+    <numFmt formatCode="#,##0" numFmtId="167"/>
   </numFmts>
   <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -653,171 +653,171 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="1" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="12" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="15" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="12" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="12" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="0" fontId="11" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="11" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="166" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="10" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="10" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="5" fillId="0" fontId="10" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="6" fillId="0" fontId="10" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="167" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="12" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="0" fontId="12" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="0" fontId="11" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="11" numFmtId="168" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="10" numFmtId="168" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="5" fillId="0" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="6" fillId="0" fontId="10" numFmtId="168" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="167" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="0" fontId="10" numFmtId="168" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="167" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="168" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="15" numFmtId="167" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -840,8 +840,8 @@
   </sheetPr>
   <dimension ref="A1:AC59"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A34" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="D57" activeCellId="0" pane="topLeft" sqref="D57"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A43" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="B57" activeCellId="0" pane="topLeft" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -878,7 +878,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="33.75" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="30.55" outlineLevel="0" r="8">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Hide "stack level too deep".
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -363,7 +363,7 @@
     <t>Шкаф холодильный СМ 110, шт</t>
   </si>
   <si>
-    <t>ИТОГО:</t>
+    <t>RESULT:</t>
   </si>
   <si>
     <t>оклад</t>
@@ -840,8 +840,8 @@
   </sheetPr>
   <dimension ref="A1:AC59"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <selection activeCell="D8" activeCellId="0" pane="topLeft" sqref="D8"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A43" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="B57" activeCellId="0" pane="topLeft" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>